<commit_message>
Dodanie Listy wszystkich spotkanych potworow i graczy. Zmiany w Sio
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>wielkośc bloku informacji o osobie to 220bitów</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>informacja czy osoba znajduje się w zasięgu widzenia znajduje się w adresie name + 0x5b flaga 36608, jeżeli nie to flaga 36735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id osoby/potwora to name -4 </t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -381,6 +384,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made Targetting Working properly and added mouse simulator
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>wielkośc bloku informacji o osobie to 220bitów</t>
   </si>
@@ -39,6 +39,21 @@
   </si>
   <si>
     <t xml:space="preserve">id osoby/potwora to name -4 </t>
+  </si>
+  <si>
+    <t>ypos to id + 28</t>
+  </si>
+  <si>
+    <t>xpos to id + 2c</t>
+  </si>
+  <si>
+    <t>mousel last X clickc Tibia.exe+581F44</t>
+  </si>
+  <si>
+    <t>mouse last Y click Tibia.exe+581F60</t>
+  </si>
+  <si>
+    <t>ground lvl to id + 24</t>
   </si>
 </sst>
 </file>
@@ -356,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -389,6 +404,31 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bugs fixed, changed auto haste to check hasted flag
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>wielkośc bloku informacji o osobie to 220bitów</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>ground lvl to id + 24</t>
+  </si>
+  <si>
+    <t>speed and protection zone are in 570410 where 64 means that character is hasted and 16384 means that character is in pz 16384+64 means is in pz and hasted</t>
   </si>
 </sst>
 </file>
@@ -374,7 +377,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,6 +422,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Message is now case sensitive
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>wielkośc bloku informacji o osobie to 220bitów</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>speed and protection zone are in 570410 where 64 means that character is hasted and 16384 means that character is in pz 16384+64 means is in pz and hasted</t>
+  </si>
+  <si>
+    <t>follow target 5815B8 flag Is 1 when yes 0 when no</t>
+  </si>
+  <si>
+    <t>actualInput is 570744 +40,40,2c</t>
   </si>
 </sst>
 </file>
@@ -374,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,6 +433,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
@@ -435,6 +446,11 @@
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Condition Action, Hash table changed to dictionary
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>wielkośc bloku informacji o osobie to 220bitów</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>actualInput is 570744 +40,40,2c</t>
+  </si>
+  <si>
+    <t>cap to xor 0x70E040 I xora</t>
+  </si>
+  <si>
+    <t>server log - najnowsza linia to 0x5C3DC0</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,36 +426,46 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>7</v>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Eating from corpse and clicking at objects in backpack. Targeter fix for diagonal option
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>wielkośc bloku informacji o osobie to 220bitów</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>odleglosc okna od gory + 8 to id okna, id eq to b5</t>
+  </si>
+  <si>
+    <t>sekundy najedzonego to 570454</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,6 +480,11 @@
         <v>15</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>